<commit_message>
Refactor PredActor to use food instead of hunger and update simulation display text
</commit_message>
<xml_diff>
--- a/data/simdata.xlsx
+++ b/data/simdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,7 +459,7 @@
         <v>20</v>
       </c>
       <c r="E2" t="n">
-        <v>3244.287252426147</v>
+        <v>3197.400331497192</v>
       </c>
     </row>
     <row r="3">
@@ -478,7 +478,7 @@
         <v>20</v>
       </c>
       <c r="E3" t="n">
-        <v>2533.116102218628</v>
+        <v>2525.983095169067</v>
       </c>
     </row>
     <row r="4">
@@ -497,7 +497,7 @@
         <v>20</v>
       </c>
       <c r="E4" t="n">
-        <v>2596.346855163574</v>
+        <v>2914.046764373779</v>
       </c>
     </row>
     <row r="5">
@@ -516,7 +516,121 @@
         <v>20</v>
       </c>
       <c r="E5" t="n">
-        <v>2567.673921585083</v>
+        <v>2470.466375350952</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>100</v>
+      </c>
+      <c r="D6" t="n">
+        <v>20</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2393.391847610474</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>100</v>
+      </c>
+      <c r="D7" t="n">
+        <v>20</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2444.068670272827</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>100</v>
+      </c>
+      <c r="D8" t="n">
+        <v>20</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2441.547632217407</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>100</v>
+      </c>
+      <c r="D9" t="n">
+        <v>20</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2436.452627182007</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>100</v>
+      </c>
+      <c r="D10" t="n">
+        <v>20</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2453.410387039185</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>100</v>
+      </c>
+      <c r="D11" t="n">
+        <v>20</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2459.134340286255</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement kill method in Actor subclasses, adjust prey/pred counts, and enhance simulation state management
</commit_message>
<xml_diff>
--- a/data/simdata.xlsx
+++ b/data/simdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -442,6 +442,11 @@
           <t>Pred</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Time(ms)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -449,17 +454,17 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>pred wins</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n">
-        <v>3197.400331497192</v>
+        <v>8273.701429367065</v>
       </c>
     </row>
     <row r="3">
@@ -472,13 +477,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>100</v>
+        <v>38</v>
       </c>
       <c r="D3" t="n">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E3" t="n">
-        <v>2525.983095169067</v>
+        <v>2480.821132659912</v>
       </c>
     </row>
     <row r="4">
@@ -491,13 +496,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>100</v>
+        <v>37</v>
       </c>
       <c r="D4" t="n">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E4" t="n">
-        <v>2914.046764373779</v>
+        <v>2461.47084236145</v>
       </c>
     </row>
     <row r="5">
@@ -510,13 +515,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>2470.466375350952</v>
+        <v>2444.170713424683</v>
       </c>
     </row>
     <row r="6">
@@ -529,13 +534,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>100</v>
+        <v>22</v>
       </c>
       <c r="D6" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E6" t="n">
-        <v>2393.391847610474</v>
+        <v>2469.356060028076</v>
       </c>
     </row>
     <row r="7">
@@ -548,13 +553,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="D7" t="n">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>2444.068670272827</v>
+        <v>2513.115882873535</v>
       </c>
     </row>
     <row r="8">
@@ -567,13 +572,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>100</v>
+        <v>44</v>
       </c>
       <c r="D8" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E8" t="n">
-        <v>2441.547632217407</v>
+        <v>2753.872632980347</v>
       </c>
     </row>
     <row r="9">
@@ -586,13 +591,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>100</v>
+        <v>49</v>
       </c>
       <c r="D9" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E9" t="n">
-        <v>2436.452627182007</v>
+        <v>2481.059789657593</v>
       </c>
     </row>
     <row r="10">
@@ -605,13 +610,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>100</v>
+        <v>59</v>
       </c>
       <c r="D10" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E10" t="n">
-        <v>2453.410387039185</v>
+        <v>2607.418537139893</v>
       </c>
     </row>
     <row r="11">
@@ -624,13 +629,298 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>100</v>
+        <v>56</v>
       </c>
       <c r="D11" t="n">
+        <v>17</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2484.508514404297</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>56</v>
+      </c>
+      <c r="D12" t="n">
+        <v>18</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2673.427581787109</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>62</v>
+      </c>
+      <c r="D13" t="n">
+        <v>19</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2567.131757736206</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>63</v>
+      </c>
+      <c r="D14" t="n">
+        <v>19</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2536.525726318359</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>61</v>
+      </c>
+      <c r="D15" t="n">
+        <v>19</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2523.674011230469</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>35</v>
+      </c>
+      <c r="D16" t="n">
+        <v>6</v>
+      </c>
+      <c r="E16" t="n">
+        <v>4960.159301757812</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>47</v>
+      </c>
+      <c r="D17" t="n">
+        <v>12</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2468.917608261108</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>61</v>
+      </c>
+      <c r="D18" t="n">
+        <v>12</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2480.092763900757</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>38</v>
+      </c>
+      <c r="D19" t="n">
+        <v>14</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2477.5230884552</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>56</v>
+      </c>
+      <c r="D20" t="n">
+        <v>15</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2709.322214126587</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>48</v>
+      </c>
+      <c r="D21" t="n">
+        <v>16</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2655.769348144531</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
         <v>20</v>
       </c>
-      <c r="E11" t="n">
-        <v>2459.134340286255</v>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>43</v>
+      </c>
+      <c r="D22" t="n">
+        <v>16</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2514.684915542603</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>49</v>
+      </c>
+      <c r="D23" t="n">
+        <v>18</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2538.419485092163</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>22</v>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>52</v>
+      </c>
+      <c r="D24" t="n">
+        <v>17</v>
+      </c>
+      <c r="E24" t="n">
+        <v>2509.968280792236</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>23</v>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>42</v>
+      </c>
+      <c r="D25" t="n">
+        <v>18</v>
+      </c>
+      <c r="E25" t="n">
+        <v>2498.693466186523</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>24</v>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>prey wins</t>
+        </is>
+      </c>
+      <c r="C26" t="n">
+        <v>61</v>
+      </c>
+      <c r="D26" t="n">
+        <v>18</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2559.166431427002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add cause of death tracking and starvation logic to Actor classes; update simulation data recording
</commit_message>
<xml_diff>
--- a/data/simdata.xlsx
+++ b/data/simdata.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Wins" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E26"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,16 @@
           <t>Time(ms)</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>prey starved</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>predator starved</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -454,17 +464,23 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>pred wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="D2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E2" t="n">
-        <v>8273.701429367065</v>
+        <v>2924.164056777954</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="3">
@@ -473,17 +489,23 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C3" t="n">
-        <v>38</v>
+        <v>90</v>
       </c>
       <c r="D3" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="E3" t="n">
-        <v>2480.821132659912</v>
+        <v>2895.161867141724</v>
+      </c>
+      <c r="F3" t="n">
+        <v>0</v>
+      </c>
+      <c r="G3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -492,17 +514,23 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C4" t="n">
-        <v>37</v>
+        <v>93</v>
       </c>
       <c r="D4" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E4" t="n">
-        <v>2461.47084236145</v>
+        <v>2513.684749603271</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="5">
@@ -511,17 +539,23 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>94</v>
       </c>
       <c r="D5" t="n">
         <v>15</v>
       </c>
       <c r="E5" t="n">
-        <v>2444.170713424683</v>
+        <v>2510.921239852905</v>
+      </c>
+      <c r="F5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -530,17 +564,23 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C6" t="n">
-        <v>22</v>
+        <v>94</v>
       </c>
       <c r="D6" t="n">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="E6" t="n">
-        <v>2469.356060028076</v>
+        <v>2490.007638931274</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -549,17 +589,23 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C7" t="n">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="D7" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E7" t="n">
-        <v>2513.115882873535</v>
+        <v>2506.988286972046</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0</v>
+      </c>
+      <c r="G7" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -568,17 +614,23 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C8" t="n">
-        <v>44</v>
+        <v>95</v>
       </c>
       <c r="D8" t="n">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E8" t="n">
-        <v>2753.872632980347</v>
+        <v>3582.927465438843</v>
+      </c>
+      <c r="F8" t="n">
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="9">
@@ -587,17 +639,23 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C9" t="n">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="D9" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E9" t="n">
-        <v>2481.059789657593</v>
+        <v>2570.085287094116</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="10">
@@ -606,17 +664,23 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C10" t="n">
-        <v>59</v>
+        <v>92</v>
       </c>
       <c r="D10" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="E10" t="n">
-        <v>2607.418537139893</v>
+        <v>2505.111694335938</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -625,17 +689,23 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>56</v>
+        <v>93</v>
       </c>
       <c r="D11" t="n">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="E11" t="n">
-        <v>2484.508514404297</v>
+        <v>2509.523630142212</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -644,17 +714,23 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="D12" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E12" t="n">
-        <v>2673.427581787109</v>
+        <v>2511.534452438354</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="13">
@@ -663,17 +739,23 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C13" t="n">
-        <v>62</v>
+        <v>95</v>
       </c>
       <c r="D13" t="n">
         <v>19</v>
       </c>
       <c r="E13" t="n">
-        <v>2567.131757736206</v>
+        <v>2499.178409576416</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="14">
@@ -682,17 +764,23 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C14" t="n">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="D14" t="n">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E14" t="n">
-        <v>2536.525726318359</v>
+        <v>2511.737108230591</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="15">
@@ -701,17 +789,23 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C15" t="n">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="D15" t="n">
         <v>19</v>
       </c>
       <c r="E15" t="n">
-        <v>2523.674011230469</v>
+        <v>2517.014026641846</v>
+      </c>
+      <c r="F15" t="n">
+        <v>0</v>
+      </c>
+      <c r="G15" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="16">
@@ -720,17 +814,23 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C16" t="n">
-        <v>35</v>
+        <v>96</v>
       </c>
       <c r="D16" t="n">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="E16" t="n">
-        <v>4960.159301757812</v>
+        <v>2521.01993560791</v>
+      </c>
+      <c r="F16" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -739,17 +839,23 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C17" t="n">
-        <v>47</v>
+        <v>95</v>
       </c>
       <c r="D17" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E17" t="n">
-        <v>2468.917608261108</v>
+        <v>2573.244094848633</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -758,17 +864,23 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C18" t="n">
-        <v>61</v>
+        <v>96</v>
       </c>
       <c r="D18" t="n">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="E18" t="n">
-        <v>2480.092763900757</v>
+        <v>2753.653764724731</v>
+      </c>
+      <c r="F18" t="n">
+        <v>0</v>
+      </c>
+      <c r="G18" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -777,17 +889,23 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C19" t="n">
-        <v>38</v>
+        <v>94</v>
       </c>
       <c r="D19" t="n">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E19" t="n">
-        <v>2477.5230884552</v>
+        <v>2544.808864593506</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0</v>
+      </c>
+      <c r="G19" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="20">
@@ -796,17 +914,23 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C20" t="n">
-        <v>56</v>
+        <v>94</v>
       </c>
       <c r="D20" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E20" t="n">
-        <v>2709.322214126587</v>
+        <v>2556.403398513794</v>
+      </c>
+      <c r="F20" t="n">
+        <v>0</v>
+      </c>
+      <c r="G20" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="21">
@@ -815,17 +939,23 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C21" t="n">
-        <v>48</v>
+        <v>94</v>
       </c>
       <c r="D21" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E21" t="n">
-        <v>2655.769348144531</v>
+        <v>2525.991678237915</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="22">
@@ -834,17 +964,23 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>43</v>
+        <v>95</v>
       </c>
       <c r="D22" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E22" t="n">
-        <v>2514.684915542603</v>
+        <v>2507.344484329224</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0</v>
+      </c>
+      <c r="G22" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -853,17 +989,23 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>49</v>
+        <v>95</v>
       </c>
       <c r="D23" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E23" t="n">
-        <v>2538.419485092163</v>
+        <v>2527.203559875488</v>
+      </c>
+      <c r="F23" t="n">
+        <v>0</v>
+      </c>
+      <c r="G23" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="24">
@@ -872,17 +1014,23 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C24" t="n">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="D24" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="E24" t="n">
-        <v>2509.968280792236</v>
+        <v>2513.854265213013</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -891,17 +1039,23 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C25" t="n">
-        <v>42</v>
+        <v>96</v>
       </c>
       <c r="D25" t="n">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E25" t="n">
-        <v>2498.693466186523</v>
+        <v>2584.317207336426</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -910,17 +1064,823 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>prey wins</t>
+          <t>wins_data</t>
         </is>
       </c>
       <c r="C26" t="n">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="D26" t="n">
+        <v>20</v>
+      </c>
+      <c r="E26" t="n">
+        <v>2573.005437850952</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>25</v>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>95</v>
+      </c>
+      <c r="D27" t="n">
+        <v>20</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2526.254177093506</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>26</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C28" t="n">
+        <v>95</v>
+      </c>
+      <c r="D28" t="n">
+        <v>20</v>
+      </c>
+      <c r="E28" t="n">
+        <v>2539.102077484131</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="n">
+        <v>27</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>95</v>
+      </c>
+      <c r="D29" t="n">
+        <v>20</v>
+      </c>
+      <c r="E29" t="n">
+        <v>2514.130353927612</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>28</v>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>95</v>
+      </c>
+      <c r="D30" t="n">
+        <v>20</v>
+      </c>
+      <c r="E30" t="n">
+        <v>2513.283967971802</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>29</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>95</v>
+      </c>
+      <c r="D31" t="n">
+        <v>20</v>
+      </c>
+      <c r="E31" t="n">
+        <v>2518.011569976807</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>30</v>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>95</v>
+      </c>
+      <c r="D32" t="n">
+        <v>20</v>
+      </c>
+      <c r="E32" t="n">
+        <v>2645.492076873779</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>31</v>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>95</v>
+      </c>
+      <c r="D33" t="n">
+        <v>20</v>
+      </c>
+      <c r="E33" t="n">
+        <v>2500.171661376953</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>32</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>95</v>
+      </c>
+      <c r="D34" t="n">
+        <v>20</v>
+      </c>
+      <c r="E34" t="n">
+        <v>2505.441665649414</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>33</v>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>95</v>
+      </c>
+      <c r="D35" t="n">
+        <v>20</v>
+      </c>
+      <c r="E35" t="n">
+        <v>2495.48077583313</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>34</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>95</v>
+      </c>
+      <c r="D36" t="n">
+        <v>20</v>
+      </c>
+      <c r="E36" t="n">
+        <v>2546.546697616577</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>95</v>
+      </c>
+      <c r="D37" t="n">
+        <v>20</v>
+      </c>
+      <c r="E37" t="n">
+        <v>2553.016185760498</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>36</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>95</v>
+      </c>
+      <c r="D38" t="n">
+        <v>20</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2521.144151687622</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>37</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C39" t="n">
+        <v>96</v>
+      </c>
+      <c r="D39" t="n">
+        <v>19</v>
+      </c>
+      <c r="E39" t="n">
+        <v>2567.018270492554</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>38</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>97</v>
+      </c>
+      <c r="D40" t="n">
         <v>18</v>
       </c>
-      <c r="E26" t="n">
-        <v>2559.166431427002</v>
+      <c r="E40" t="n">
+        <v>2536.957740783691</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>39</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>96</v>
+      </c>
+      <c r="D41" t="n">
+        <v>19</v>
+      </c>
+      <c r="E41" t="n">
+        <v>2530.840396881104</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>40</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>97</v>
+      </c>
+      <c r="D42" t="n">
+        <v>18</v>
+      </c>
+      <c r="E42" t="n">
+        <v>2531.039237976074</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>41</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>93</v>
+      </c>
+      <c r="D43" t="n">
+        <v>19</v>
+      </c>
+      <c r="E43" t="n">
+        <v>2491.824150085449</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>42</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>95</v>
+      </c>
+      <c r="D44" t="n">
+        <v>19</v>
+      </c>
+      <c r="E44" t="n">
+        <v>2478.105783462524</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
+        <v>43</v>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>95</v>
+      </c>
+      <c r="D45" t="n">
+        <v>19</v>
+      </c>
+      <c r="E45" t="n">
+        <v>2498.443603515625</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>44</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>96</v>
+      </c>
+      <c r="D46" t="n">
+        <v>19</v>
+      </c>
+      <c r="E46" t="n">
+        <v>2541.606664657593</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0</v>
+      </c>
+      <c r="G46" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>45</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>97</v>
+      </c>
+      <c r="D47" t="n">
+        <v>20</v>
+      </c>
+      <c r="E47" t="n">
+        <v>2529.894351959229</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>46</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>97</v>
+      </c>
+      <c r="D48" t="n">
+        <v>20</v>
+      </c>
+      <c r="E48" t="n">
+        <v>2524.283647537231</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0</v>
+      </c>
+      <c r="G48" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>47</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>98</v>
+      </c>
+      <c r="D49" t="n">
+        <v>19</v>
+      </c>
+      <c r="E49" t="n">
+        <v>2546.886205673218</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="n">
+        <v>48</v>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C50" t="n">
+        <v>96</v>
+      </c>
+      <c r="D50" t="n">
+        <v>20</v>
+      </c>
+      <c r="E50" t="n">
+        <v>2516.337633132935</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0</v>
+      </c>
+      <c r="G50" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="n">
+        <v>49</v>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>97</v>
+      </c>
+      <c r="D51" t="n">
+        <v>20</v>
+      </c>
+      <c r="E51" t="n">
+        <v>2478.877782821655</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0</v>
+      </c>
+      <c r="G51" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="n">
+        <v>50</v>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>97</v>
+      </c>
+      <c r="D52" t="n">
+        <v>20</v>
+      </c>
+      <c r="E52" t="n">
+        <v>2538.672924041748</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="n">
+        <v>51</v>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>98</v>
+      </c>
+      <c r="D53" t="n">
+        <v>19</v>
+      </c>
+      <c r="E53" t="n">
+        <v>2508.635997772217</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="n">
+        <v>52</v>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>97</v>
+      </c>
+      <c r="D54" t="n">
+        <v>20</v>
+      </c>
+      <c r="E54" t="n">
+        <v>2517.949104309082</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0</v>
+      </c>
+      <c r="G54" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="n">
+        <v>53</v>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>97</v>
+      </c>
+      <c r="D55" t="n">
+        <v>20</v>
+      </c>
+      <c r="E55" t="n">
+        <v>2510.123014450073</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0</v>
+      </c>
+      <c r="G55" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="n">
+        <v>54</v>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>98</v>
+      </c>
+      <c r="D56" t="n">
+        <v>20</v>
+      </c>
+      <c r="E56" t="n">
+        <v>2528.88560295105</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0</v>
+      </c>
+      <c r="G56" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="n">
+        <v>55</v>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>98</v>
+      </c>
+      <c r="D57" t="n">
+        <v>20</v>
+      </c>
+      <c r="E57" t="n">
+        <v>2537.395000457764</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="n">
+        <v>56</v>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>98</v>
+      </c>
+      <c r="D58" t="n">
+        <v>20</v>
+      </c>
+      <c r="E58" t="n">
+        <v>2500.885725021362</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Refactor Actor and subclasses to implement food management, adjust hunger thresholds, and enhance scoring logic; update cell drawing based on food levels
</commit_message>
<xml_diff>
--- a/data/simdata.xlsx
+++ b/data/simdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G58"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,13 +468,13 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="D2" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E2" t="n">
-        <v>2924.164056777954</v>
+        <v>2854.290246963501</v>
       </c>
       <c r="F2" t="n">
         <v>0</v>
@@ -493,13 +493,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>90</v>
+        <v>49</v>
       </c>
       <c r="D3" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E3" t="n">
-        <v>2895.161867141724</v>
+        <v>3374.71079826355</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -518,13 +518,13 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>93</v>
+        <v>57</v>
       </c>
       <c r="D4" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E4" t="n">
-        <v>2513.684749603271</v>
+        <v>3491.153955459595</v>
       </c>
       <c r="F4" t="n">
         <v>0</v>
@@ -543,13 +543,13 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="D5" t="n">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E5" t="n">
-        <v>2510.921239852905</v>
+        <v>3469.091176986694</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -568,13 +568,13 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>94</v>
+        <v>68</v>
       </c>
       <c r="D6" t="n">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="E6" t="n">
-        <v>2490.007638931274</v>
+        <v>3477.364301681519</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -593,13 +593,13 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>95</v>
+        <v>73</v>
       </c>
       <c r="D7" t="n">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E7" t="n">
-        <v>2506.988286972046</v>
+        <v>3500.184535980225</v>
       </c>
       <c r="F7" t="n">
         <v>0</v>
@@ -618,13 +618,13 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>95</v>
+        <v>79</v>
       </c>
       <c r="D8" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="E8" t="n">
-        <v>3582.927465438843</v>
+        <v>2777.769565582275</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -643,13 +643,13 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="D9" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E9" t="n">
-        <v>2570.085287094116</v>
+        <v>2437.819242477417</v>
       </c>
       <c r="F9" t="n">
         <v>0</v>
@@ -668,13 +668,13 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="D10" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E10" t="n">
-        <v>2505.111694335938</v>
+        <v>2425.56095123291</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -693,13 +693,13 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="D11" t="n">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="E11" t="n">
-        <v>2509.523630142212</v>
+        <v>2478.605508804321</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -718,13 +718,13 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="D12" t="n">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="E12" t="n">
-        <v>2511.534452438354</v>
+        <v>2467.833995819092</v>
       </c>
       <c r="F12" t="n">
         <v>0</v>
@@ -743,13 +743,13 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>95</v>
+        <v>82</v>
       </c>
       <c r="D13" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E13" t="n">
-        <v>2499.178409576416</v>
+        <v>2496.679067611694</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -768,13 +768,13 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="D14" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E14" t="n">
-        <v>2511.737108230591</v>
+        <v>2461.416959762573</v>
       </c>
       <c r="F14" t="n">
         <v>0</v>
@@ -793,13 +793,13 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="D15" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E15" t="n">
-        <v>2517.014026641846</v>
+        <v>2447.9820728302</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -818,13 +818,13 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D16" t="n">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E16" t="n">
-        <v>2521.01993560791</v>
+        <v>2436.282157897949</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -843,13 +843,13 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D17" t="n">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E17" t="n">
-        <v>2573.244094848633</v>
+        <v>2550.219774246216</v>
       </c>
       <c r="F17" t="n">
         <v>0</v>
@@ -868,13 +868,13 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D18" t="n">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="E18" t="n">
-        <v>2753.653764724731</v>
+        <v>2463.279247283936</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -893,13 +893,13 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="D19" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E19" t="n">
-        <v>2544.808864593506</v>
+        <v>2444.960117340088</v>
       </c>
       <c r="F19" t="n">
         <v>0</v>
@@ -918,13 +918,13 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="D20" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E20" t="n">
-        <v>2556.403398513794</v>
+        <v>2455.043077468872</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -943,13 +943,13 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="D21" t="n">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="E21" t="n">
-        <v>2525.991678237915</v>
+        <v>2449.816703796387</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -968,13 +968,13 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D22" t="n">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E22" t="n">
-        <v>2507.344484329224</v>
+        <v>2461.83443069458</v>
       </c>
       <c r="F22" t="n">
         <v>0</v>
@@ -993,13 +993,13 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D23" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E23" t="n">
-        <v>2527.203559875488</v>
+        <v>2494.901180267334</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -1018,13 +1018,13 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D24" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E24" t="n">
-        <v>2513.854265213013</v>
+        <v>2500.065088272095</v>
       </c>
       <c r="F24" t="n">
         <v>0</v>
@@ -1043,13 +1043,13 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="D25" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E25" t="n">
-        <v>2584.317207336426</v>
+        <v>2494.084358215332</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -1068,13 +1068,13 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="D26" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E26" t="n">
-        <v>2573.005437850952</v>
+        <v>2460.748910903931</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -1093,13 +1093,13 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="D27" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E27" t="n">
-        <v>2526.254177093506</v>
+        <v>2483.832836151123</v>
       </c>
       <c r="F27" t="n">
         <v>0</v>
@@ -1118,13 +1118,13 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D28" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E28" t="n">
-        <v>2539.102077484131</v>
+        <v>3773.667335510254</v>
       </c>
       <c r="F28" t="n">
         <v>0</v>
@@ -1143,13 +1143,13 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D29" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E29" t="n">
-        <v>2514.130353927612</v>
+        <v>2492.933034896851</v>
       </c>
       <c r="F29" t="n">
         <v>0</v>
@@ -1168,13 +1168,13 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D30" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E30" t="n">
-        <v>2513.283967971802</v>
+        <v>2464.917421340942</v>
       </c>
       <c r="F30" t="n">
         <v>0</v>
@@ -1193,13 +1193,13 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D31" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E31" t="n">
-        <v>2518.011569976807</v>
+        <v>2518.134117126465</v>
       </c>
       <c r="F31" t="n">
         <v>0</v>
@@ -1218,13 +1218,13 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D32" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E32" t="n">
-        <v>2645.492076873779</v>
+        <v>2447.538375854492</v>
       </c>
       <c r="F32" t="n">
         <v>0</v>
@@ -1243,13 +1243,13 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D33" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E33" t="n">
-        <v>2500.171661376953</v>
+        <v>2465.011119842529</v>
       </c>
       <c r="F33" t="n">
         <v>0</v>
@@ -1268,13 +1268,13 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D34" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E34" t="n">
-        <v>2505.441665649414</v>
+        <v>2468.804836273193</v>
       </c>
       <c r="F34" t="n">
         <v>0</v>
@@ -1293,13 +1293,13 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="D35" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E35" t="n">
-        <v>2495.48077583313</v>
+        <v>2474.011898040771</v>
       </c>
       <c r="F35" t="n">
         <v>0</v>
@@ -1318,13 +1318,13 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D36" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E36" t="n">
-        <v>2546.546697616577</v>
+        <v>2438.58814239502</v>
       </c>
       <c r="F36" t="n">
         <v>0</v>
@@ -1343,13 +1343,13 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D37" t="n">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="E37" t="n">
-        <v>2553.016185760498</v>
+        <v>2464.380264282227</v>
       </c>
       <c r="F37" t="n">
         <v>0</v>
@@ -1368,13 +1368,13 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D38" t="n">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E38" t="n">
-        <v>2521.144151687622</v>
+        <v>2481.318473815918</v>
       </c>
       <c r="F38" t="n">
         <v>0</v>
@@ -1393,13 +1393,13 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D39" t="n">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E39" t="n">
-        <v>2567.018270492554</v>
+        <v>2463.472127914429</v>
       </c>
       <c r="F39" t="n">
         <v>0</v>
@@ -1418,13 +1418,13 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D40" t="n">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E40" t="n">
-        <v>2536.957740783691</v>
+        <v>2474.099636077881</v>
       </c>
       <c r="F40" t="n">
         <v>0</v>
@@ -1443,13 +1443,13 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D41" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E41" t="n">
-        <v>2530.840396881104</v>
+        <v>2464.581727981567</v>
       </c>
       <c r="F41" t="n">
         <v>0</v>
@@ -1468,13 +1468,13 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D42" t="n">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E42" t="n">
-        <v>2531.039237976074</v>
+        <v>2509.955406188965</v>
       </c>
       <c r="F42" t="n">
         <v>0</v>
@@ -1496,10 +1496,10 @@
         <v>93</v>
       </c>
       <c r="D43" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E43" t="n">
-        <v>2491.824150085449</v>
+        <v>2491.349458694458</v>
       </c>
       <c r="F43" t="n">
         <v>0</v>
@@ -1518,13 +1518,13 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D44" t="n">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E44" t="n">
-        <v>2478.105783462524</v>
+        <v>2484.604120254517</v>
       </c>
       <c r="F44" t="n">
         <v>0</v>
@@ -1543,13 +1543,13 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="D45" t="n">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E45" t="n">
-        <v>2498.443603515625</v>
+        <v>2485.413074493408</v>
       </c>
       <c r="F45" t="n">
         <v>0</v>
@@ -1568,13 +1568,13 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D46" t="n">
         <v>19</v>
       </c>
       <c r="E46" t="n">
-        <v>2541.606664657593</v>
+        <v>2466.079235076904</v>
       </c>
       <c r="F46" t="n">
         <v>0</v>
@@ -1593,13 +1593,13 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D47" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E47" t="n">
-        <v>2529.894351959229</v>
+        <v>2472.551584243774</v>
       </c>
       <c r="F47" t="n">
         <v>0</v>
@@ -1618,13 +1618,13 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D48" t="n">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E48" t="n">
-        <v>2524.283647537231</v>
+        <v>2490.83948135376</v>
       </c>
       <c r="F48" t="n">
         <v>0</v>
@@ -1643,13 +1643,13 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D49" t="n">
         <v>19</v>
       </c>
       <c r="E49" t="n">
-        <v>2546.886205673218</v>
+        <v>2509.913206100464</v>
       </c>
       <c r="F49" t="n">
         <v>0</v>
@@ -1668,13 +1668,13 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D50" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E50" t="n">
-        <v>2516.337633132935</v>
+        <v>2462.328910827637</v>
       </c>
       <c r="F50" t="n">
         <v>0</v>
@@ -1693,193 +1693,18 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D51" t="n">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E51" t="n">
-        <v>2478.877782821655</v>
+        <v>2478.613615036011</v>
       </c>
       <c r="F51" t="n">
         <v>0</v>
       </c>
       <c r="G51" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="n">
-        <v>50</v>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>97</v>
-      </c>
-      <c r="D52" t="n">
-        <v>20</v>
-      </c>
-      <c r="E52" t="n">
-        <v>2538.672924041748</v>
-      </c>
-      <c r="F52" t="n">
-        <v>0</v>
-      </c>
-      <c r="G52" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="n">
-        <v>51</v>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C53" t="n">
-        <v>98</v>
-      </c>
-      <c r="D53" t="n">
-        <v>19</v>
-      </c>
-      <c r="E53" t="n">
-        <v>2508.635997772217</v>
-      </c>
-      <c r="F53" t="n">
-        <v>0</v>
-      </c>
-      <c r="G53" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="n">
-        <v>52</v>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C54" t="n">
-        <v>97</v>
-      </c>
-      <c r="D54" t="n">
-        <v>20</v>
-      </c>
-      <c r="E54" t="n">
-        <v>2517.949104309082</v>
-      </c>
-      <c r="F54" t="n">
-        <v>0</v>
-      </c>
-      <c r="G54" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="n">
-        <v>53</v>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C55" t="n">
-        <v>97</v>
-      </c>
-      <c r="D55" t="n">
-        <v>20</v>
-      </c>
-      <c r="E55" t="n">
-        <v>2510.123014450073</v>
-      </c>
-      <c r="F55" t="n">
-        <v>0</v>
-      </c>
-      <c r="G55" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="n">
-        <v>54</v>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C56" t="n">
-        <v>98</v>
-      </c>
-      <c r="D56" t="n">
-        <v>20</v>
-      </c>
-      <c r="E56" t="n">
-        <v>2528.88560295105</v>
-      </c>
-      <c r="F56" t="n">
-        <v>0</v>
-      </c>
-      <c r="G56" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="n">
-        <v>55</v>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C57" t="n">
-        <v>98</v>
-      </c>
-      <c r="D57" t="n">
-        <v>20</v>
-      </c>
-      <c r="E57" t="n">
-        <v>2537.395000457764</v>
-      </c>
-      <c r="F57" t="n">
-        <v>0</v>
-      </c>
-      <c r="G57" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="n">
-        <v>56</v>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C58" t="n">
-        <v>98</v>
-      </c>
-      <c r="D58" t="n">
-        <v>20</v>
-      </c>
-      <c r="E58" t="n">
-        <v>2500.885725021362</v>
-      </c>
-      <c r="F58" t="n">
-        <v>0</v>
-      </c>
-      <c r="G58" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update .gitignore, enhance VSCode launch configuration, and refactor serialization methods in Actor and Cell classes; adjust simulation state management and save logic
</commit_message>
<xml_diff>
--- a/data/simdata.xlsx
+++ b/data/simdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,10 +474,10 @@
         <v>20</v>
       </c>
       <c r="E2" t="n">
-        <v>5475.902795791626</v>
+        <v>2199.702739715576</v>
       </c>
       <c r="F2" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -493,13 +493,13 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D3" t="n">
         <v>3</v>
       </c>
       <c r="E3" t="n">
-        <v>4989.621162414551</v>
+        <v>1629.07862663269</v>
       </c>
       <c r="F3" t="n">
         <v>8</v>
@@ -518,19 +518,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D4" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>4996.731996536255</v>
+        <v>1659.323692321777</v>
       </c>
       <c r="F4" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5">
@@ -543,19 +543,19 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D5" t="n">
+        <v>3</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1700.087308883667</v>
+      </c>
+      <c r="F5" t="n">
         <v>4</v>
       </c>
-      <c r="E5" t="n">
-        <v>4989.547252655029</v>
-      </c>
-      <c r="F5" t="n">
-        <v>7</v>
-      </c>
       <c r="G5" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6">
@@ -568,19 +568,19 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
+        <v>1690.253496170044</v>
+      </c>
+      <c r="F6" t="n">
         <v>4</v>
       </c>
-      <c r="E6" t="n">
-        <v>4997.479200363159</v>
-      </c>
-      <c r="F6" t="n">
-        <v>6</v>
-      </c>
       <c r="G6" t="n">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7">
@@ -593,19 +593,19 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="D7" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E7" t="n">
-        <v>4991.931915283203</v>
+        <v>1680.027484893799</v>
       </c>
       <c r="F7" t="n">
         <v>3</v>
       </c>
       <c r="G7" t="n">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
@@ -624,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="E8" t="n">
-        <v>5000.040531158447</v>
+        <v>1672.077894210815</v>
       </c>
       <c r="F8" t="n">
         <v>4</v>
@@ -643,19 +643,19 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E9" t="n">
-        <v>4992.088556289673</v>
+        <v>1645.671606063843</v>
       </c>
       <c r="F9" t="n">
         <v>4</v>
       </c>
       <c r="G9" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10">
@@ -668,19 +668,19 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="D10" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E10" t="n">
-        <v>4999.223947525024</v>
+        <v>1636.59143447876</v>
       </c>
       <c r="F10" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G10" t="n">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11">
@@ -696,141 +696,16 @@
         <v>43</v>
       </c>
       <c r="D11" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11" t="n">
-        <v>4992.521286010742</v>
+        <v>1726.107835769653</v>
       </c>
       <c r="F11" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G11" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="n">
-        <v>10</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C12" t="n">
-        <v>43</v>
-      </c>
-      <c r="D12" t="n">
-        <v>4</v>
-      </c>
-      <c r="E12" t="n">
-        <v>4999.212265014648</v>
-      </c>
-      <c r="F12" t="n">
-        <v>4</v>
-      </c>
-      <c r="G12" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="n">
-        <v>11</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C13" t="n">
-        <v>43</v>
-      </c>
-      <c r="D13" t="n">
-        <v>6</v>
-      </c>
-      <c r="E13" t="n">
-        <v>4990.557670593262</v>
-      </c>
-      <c r="F13" t="n">
-        <v>4</v>
-      </c>
-      <c r="G13" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>12</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C14" t="n">
-        <v>43</v>
-      </c>
-      <c r="D14" t="n">
-        <v>6</v>
-      </c>
-      <c r="E14" t="n">
-        <v>4991.695165634155</v>
-      </c>
-      <c r="F14" t="n">
-        <v>4</v>
-      </c>
-      <c r="G14" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
         <v>13</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C15" t="n">
-        <v>42</v>
-      </c>
-      <c r="D15" t="n">
-        <v>6</v>
-      </c>
-      <c r="E15" t="n">
-        <v>4998.230218887329</v>
-      </c>
-      <c r="F15" t="n">
-        <v>4</v>
-      </c>
-      <c r="G15" t="n">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>14</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C16" t="n">
-        <v>43</v>
-      </c>
-      <c r="D16" t="n">
-        <v>6</v>
-      </c>
-      <c r="E16" t="n">
-        <v>4994.305849075317</v>
-      </c>
-      <c r="F16" t="n">
-        <v>5</v>
-      </c>
-      <c r="G16" t="n">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement replay functionality in SimState and add Replay script; adjust prey count and maximum generations for simulation
</commit_message>
<xml_diff>
--- a/data/simdata.xlsx
+++ b/data/simdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>37</v>
+        <v>72</v>
       </c>
       <c r="D2" t="n">
         <v>20</v>
       </c>
       <c r="E2" t="n">
-        <v>2199.702739715576</v>
+        <v>3041.325569152832</v>
       </c>
       <c r="F2" t="n">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="G2" t="n">
         <v>0</v>
@@ -493,219 +493,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>38</v>
+        <v>68</v>
       </c>
       <c r="D3" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E3" t="n">
-        <v>1629.07862663269</v>
+        <v>2740.487575531006</v>
       </c>
       <c r="F3" t="n">
-        <v>8</v>
+        <v>26</v>
       </c>
       <c r="G3" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="n">
-        <v>2</v>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C4" t="n">
-        <v>41</v>
-      </c>
-      <c r="D4" t="n">
-        <v>5</v>
-      </c>
-      <c r="E4" t="n">
-        <v>1659.323692321777</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4</v>
-      </c>
-      <c r="G4" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>43</v>
-      </c>
-      <c r="D5" t="n">
-        <v>3</v>
-      </c>
-      <c r="E5" t="n">
-        <v>1700.087308883667</v>
-      </c>
-      <c r="F5" t="n">
-        <v>4</v>
-      </c>
-      <c r="G5" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="n">
-        <v>4</v>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C6" t="n">
-        <v>43</v>
-      </c>
-      <c r="D6" t="n">
-        <v>3</v>
-      </c>
-      <c r="E6" t="n">
-        <v>1690.253496170044</v>
-      </c>
-      <c r="F6" t="n">
-        <v>4</v>
-      </c>
-      <c r="G6" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="n">
-        <v>5</v>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C7" t="n">
-        <v>44</v>
-      </c>
-      <c r="D7" t="n">
-        <v>3</v>
-      </c>
-      <c r="E7" t="n">
-        <v>1680.027484893799</v>
-      </c>
-      <c r="F7" t="n">
-        <v>3</v>
-      </c>
-      <c r="G7" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="n">
-        <v>6</v>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C8" t="n">
-        <v>43</v>
-      </c>
-      <c r="D8" t="n">
-        <v>3</v>
-      </c>
-      <c r="E8" t="n">
-        <v>1672.077894210815</v>
-      </c>
-      <c r="F8" t="n">
-        <v>4</v>
-      </c>
-      <c r="G8" t="n">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="n">
-        <v>7</v>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C9" t="n">
-        <v>43</v>
-      </c>
-      <c r="D9" t="n">
-        <v>4</v>
-      </c>
-      <c r="E9" t="n">
-        <v>1645.671606063843</v>
-      </c>
-      <c r="F9" t="n">
-        <v>4</v>
-      </c>
-      <c r="G9" t="n">
         <v>16</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="n">
-        <v>8</v>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C10" t="n">
-        <v>44</v>
-      </c>
-      <c r="D10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E10" t="n">
-        <v>1636.59143447876</v>
-      </c>
-      <c r="F10" t="n">
-        <v>3</v>
-      </c>
-      <c r="G10" t="n">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="n">
-        <v>9</v>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C11" t="n">
-        <v>43</v>
-      </c>
-      <c r="D11" t="n">
-        <v>7</v>
-      </c>
-      <c r="E11" t="n">
-        <v>1726.107835769653</v>
-      </c>
-      <c r="F11" t="n">
-        <v>3</v>
-      </c>
-      <c r="G11" t="n">
-        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Reduce MaxActions in SimState from 100 to 50 for improved simulation performance
</commit_message>
<xml_diff>
--- a/data/simdata.xlsx
+++ b/data/simdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,19 +468,94 @@
         </is>
       </c>
       <c r="C2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" t="n">
+        <v>4</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4878.515958786011</v>
+      </c>
+      <c r="F2" t="n">
+        <v>92</v>
+      </c>
+      <c r="G2" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" t="n">
+        <v>4</v>
+      </c>
+      <c r="E3" t="n">
+        <v>4468.364238739014</v>
+      </c>
+      <c r="F3" t="n">
+        <v>91</v>
+      </c>
+      <c r="G3" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
         <v>2</v>
       </c>
-      <c r="D2" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" t="n">
         <v>5</v>
       </c>
-      <c r="E2" t="n">
-        <v>5196.133852005005</v>
-      </c>
-      <c r="F2" t="n">
-        <v>90</v>
-      </c>
-      <c r="G2" t="n">
+      <c r="E4" t="n">
+        <v>4360.931396484375</v>
+      </c>
+      <c r="F4" t="n">
+        <v>87</v>
+      </c>
+      <c r="G4" t="n">
         <v>15</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" t="n">
+        <v>4</v>
+      </c>
+      <c r="E5" t="n">
+        <v>4282.888650894165</v>
+      </c>
+      <c r="F5" t="n">
+        <v>89</v>
+      </c>
+      <c r="G5" t="n">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ActorType and Moves enums; refactor action handling in Actor, PredActor, and PreyActor classes
</commit_message>
<xml_diff>
--- a/data/simdata.xlsx
+++ b/data/simdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,19 +468,19 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>87</v>
       </c>
       <c r="D2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>4878.515958786011</v>
+        <v>3379.408121109009</v>
       </c>
       <c r="F2" t="n">
-        <v>92</v>
+        <v>6</v>
       </c>
       <c r="G2" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3">
@@ -493,19 +493,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>89</v>
       </c>
       <c r="D3" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>4468.364238739014</v>
+        <v>2532.006978988647</v>
       </c>
       <c r="F3" t="n">
-        <v>91</v>
+        <v>5</v>
       </c>
       <c r="G3" t="n">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
@@ -518,44 +518,19 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>4</v>
+        <v>90</v>
       </c>
       <c r="D4" t="n">
         <v>5</v>
       </c>
       <c r="E4" t="n">
-        <v>4360.931396484375</v>
+        <v>2782.976865768433</v>
       </c>
       <c r="F4" t="n">
-        <v>87</v>
+        <v>4</v>
       </c>
       <c r="G4" t="n">
         <v>15</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>3</v>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>wins_data</t>
-        </is>
-      </c>
-      <c r="C5" t="n">
-        <v>3</v>
-      </c>
-      <c r="D5" t="n">
-        <v>4</v>
-      </c>
-      <c r="E5" t="n">
-        <v>4282.888650894165</v>
-      </c>
-      <c r="F5" t="n">
-        <v>89</v>
-      </c>
-      <c r="G5" t="n">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Implement food search and threat sensing in Actor subclasses; refactor movement logic for better decision-making
</commit_message>
<xml_diff>
--- a/data/simdata.xlsx
+++ b/data/simdata.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -468,16 +468,16 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D2" t="n">
         <v>5</v>
       </c>
       <c r="E2" t="n">
-        <v>3379.408121109009</v>
+        <v>3126.129388809204</v>
       </c>
       <c r="F2" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G2" t="n">
         <v>15</v>
@@ -493,19 +493,19 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E3" t="n">
-        <v>2532.006978988647</v>
+        <v>2639.851808547974</v>
       </c>
       <c r="F3" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G3" t="n">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4">
@@ -521,16 +521,491 @@
         <v>90</v>
       </c>
       <c r="D4" t="n">
+        <v>10</v>
+      </c>
+      <c r="E4" t="n">
+        <v>2681.691646575928</v>
+      </c>
+      <c r="F4" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>90</v>
+      </c>
+      <c r="D5" t="n">
+        <v>8</v>
+      </c>
+      <c r="E5" t="n">
+        <v>2624.805212020874</v>
+      </c>
+      <c r="F5" t="n">
+        <v>3</v>
+      </c>
+      <c r="G5" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C6" t="n">
+        <v>89</v>
+      </c>
+      <c r="D6" t="n">
+        <v>13</v>
+      </c>
+      <c r="E6" t="n">
+        <v>2650.022268295288</v>
+      </c>
+      <c r="F6" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
         <v>5</v>
       </c>
-      <c r="E4" t="n">
-        <v>2782.976865768433</v>
-      </c>
-      <c r="F4" t="n">
-        <v>4</v>
-      </c>
-      <c r="G4" t="n">
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>90</v>
+      </c>
+      <c r="D7" t="n">
+        <v>9</v>
+      </c>
+      <c r="E7" t="n">
+        <v>2633.105278015137</v>
+      </c>
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>92</v>
+      </c>
+      <c r="D8" t="n">
+        <v>10</v>
+      </c>
+      <c r="E8" t="n">
+        <v>2665.648937225342</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>91</v>
+      </c>
+      <c r="D9" t="n">
+        <v>12</v>
+      </c>
+      <c r="E9" t="n">
+        <v>2632.755041122437</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>90</v>
+      </c>
+      <c r="D10" t="n">
+        <v>12</v>
+      </c>
+      <c r="E10" t="n">
+        <v>2627.527475357056</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>91</v>
+      </c>
+      <c r="D11" t="n">
+        <v>9</v>
+      </c>
+      <c r="E11" t="n">
+        <v>2648.579359054565</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>91</v>
+      </c>
+      <c r="D12" t="n">
+        <v>12</v>
+      </c>
+      <c r="E12" t="n">
+        <v>2614.293813705444</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>90</v>
+      </c>
+      <c r="D13" t="n">
+        <v>13</v>
+      </c>
+      <c r="E13" t="n">
+        <v>2633.073806762695</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C14" t="n">
+        <v>93</v>
+      </c>
+      <c r="D14" t="n">
+        <v>12</v>
+      </c>
+      <c r="E14" t="n">
+        <v>2650.115728378296</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C15" t="n">
+        <v>91</v>
+      </c>
+      <c r="D15" t="n">
+        <v>14</v>
+      </c>
+      <c r="E15" t="n">
+        <v>2613.082647323608</v>
+      </c>
+      <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>91</v>
+      </c>
+      <c r="D16" t="n">
         <v>15</v>
+      </c>
+      <c r="E16" t="n">
+        <v>2673.084735870361</v>
+      </c>
+      <c r="F16" t="n">
+        <v>1</v>
+      </c>
+      <c r="G16" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C17" t="n">
+        <v>92</v>
+      </c>
+      <c r="D17" t="n">
+        <v>12</v>
+      </c>
+      <c r="E17" t="n">
+        <v>2675.118923187256</v>
+      </c>
+      <c r="F17" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>16</v>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>93</v>
+      </c>
+      <c r="D18" t="n">
+        <v>13</v>
+      </c>
+      <c r="E18" t="n">
+        <v>2635.033130645752</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>17</v>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>93</v>
+      </c>
+      <c r="D19" t="n">
+        <v>12</v>
+      </c>
+      <c r="E19" t="n">
+        <v>2617.598533630371</v>
+      </c>
+      <c r="F19" t="n">
+        <v>1</v>
+      </c>
+      <c r="G19" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>18</v>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>90</v>
+      </c>
+      <c r="D20" t="n">
+        <v>13</v>
+      </c>
+      <c r="E20" t="n">
+        <v>2600.1136302948</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1</v>
+      </c>
+      <c r="G20" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>19</v>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>93</v>
+      </c>
+      <c r="D21" t="n">
+        <v>13</v>
+      </c>
+      <c r="E21" t="n">
+        <v>2647.555112838745</v>
+      </c>
+      <c r="F21" t="n">
+        <v>0</v>
+      </c>
+      <c r="G21" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>20</v>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>93</v>
+      </c>
+      <c r="D22" t="n">
+        <v>13</v>
+      </c>
+      <c r="E22" t="n">
+        <v>2670.164346694946</v>
+      </c>
+      <c r="F22" t="n">
+        <v>1</v>
+      </c>
+      <c r="G22" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="n">
+        <v>21</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>wins_data</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>93</v>
+      </c>
+      <c r="D23" t="n">
+        <v>13</v>
+      </c>
+      <c r="E23" t="n">
+        <v>2620.767116546631</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1</v>
+      </c>
+      <c r="G23" t="n">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>